<commit_message>
feature: use regex to extract a part organization name
</commit_message>
<xml_diff>
--- a/tests/data/non_counter/my-date-metric-based.xlsx
+++ b/tests/data/non_counter/my-date-metric-based.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t xml:space="preserve">Extra</t>
   </si>
@@ -50,97 +50,13 @@
     <t xml:space="preserve">PROD</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MYCONS </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Org1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MYCONS </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">–</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Org2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MYCONS </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">–</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Org3</t>
-    </r>
+    <t xml:space="preserve">MYCONS - Org1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYCONS - Org2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYCONS - Org3</t>
   </si>
   <si>
     <t xml:space="preserve">Month</t>
@@ -150,6 +66,12 @@
   </si>
   <si>
     <t xml:space="preserve">Views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYCONS – Org2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYCONS – Org3</t>
   </si>
 </sst>
 </file>
@@ -160,7 +82,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mmm\-yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -191,12 +113,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -240,8 +156,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -273,122 +193,122 @@
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -490,177 +410,177 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>43850</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>43881</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>43910</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="n">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <v>43850</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="n">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>43881</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="n">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <v>43910</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="n">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <v>43850</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="n">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="n">
         <v>43881</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="n">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="n">
         <v>43910</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>